<commit_message>
ADDING SD.PAGES ON PROGRAM
</commit_message>
<xml_diff>
--- a/Team14_LMS_UI_TestingSprinters/src/test/resources/TestData/LMSTestData.xlsx
+++ b/Team14_LMS_UI_TestingSprinters/src/test/resources/TestData/LMSTestData.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumal\eclipse-workspace\LMS_seleniumPhase2\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumal\git\Test14_TestingSprinters_LMS_UI\Team14_LMS_UI_TestingSprinters\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B42CA9-578E-42C7-9D04-9F8B5D4F5377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0416739-78A9-4FA5-8A6F-7C9F584AEF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="3" r:id="rId1"/>
-    <sheet name="BatchSheet" sheetId="1" r:id="rId2"/>
+    <sheet name="Manage Program" sheetId="4" r:id="rId2"/>
+    <sheet name="Add Program" sheetId="5" r:id="rId3"/>
+    <sheet name="BatchSheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -161,13 +163,127 @@
   </si>
   <si>
     <t>UIHackathon@02</t>
+  </si>
+  <si>
+    <t>KeyOption</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>descriptionfrPrgrm</t>
+  </si>
+  <si>
+    <t>prgrmStatus</t>
+  </si>
+  <si>
+    <t>SearchProgramByInvalidName</t>
+  </si>
+  <si>
+    <t>%%^&amp;%</t>
+  </si>
+  <si>
+    <t>SearchProgramByName</t>
+  </si>
+  <si>
+    <t>SDET</t>
+  </si>
+  <si>
+    <t>SearchProgramByDescription</t>
+  </si>
+  <si>
+    <t>learn API</t>
+  </si>
+  <si>
+    <t>SearchProgramByStatus</t>
+  </si>
+  <si>
+    <t>EnterOnlyProgramName</t>
+  </si>
+  <si>
+    <t>EnterOnlyProgramDesc</t>
+  </si>
+  <si>
+    <t>EnterOnlyProgramStatus</t>
+  </si>
+  <si>
+    <t>InvalidProgramDetails</t>
+  </si>
+  <si>
+    <t>*&amp;^&amp;234</t>
+  </si>
+  <si>
+    <t>74823&amp;%&amp;</t>
+  </si>
+  <si>
+    <t>ValidProgramDetails</t>
+  </si>
+  <si>
+    <t>UpdateProgramName</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>UpdateProgramDescription</t>
+  </si>
+  <si>
+    <t>SQL JAVA</t>
+  </si>
+  <si>
+    <t>Empty_form_submission</t>
+  </si>
+  <si>
+    <t>Enter_only_Program_Name</t>
+  </si>
+  <si>
+    <t>Enter_only_Program_Description</t>
+  </si>
+  <si>
+    <t>Select_Status_only</t>
+  </si>
+  <si>
+    <t>Validate_invalid_values_on_the_text_column</t>
+  </si>
+  <si>
+    <t>Validate_Save_button_on_Program_Details_form</t>
+  </si>
+  <si>
+    <t>Validate_Cancel_button_on_Program_Details_form</t>
+  </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>SDET Description</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Validate_Close(X)_icon_on_Program_Details_form</t>
+  </si>
+  <si>
+    <t>Save_Valid_Program_Data</t>
+  </si>
+  <si>
+    <t>SDET_T14_DESC</t>
+  </si>
+  <si>
+    <t>SDETT14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +423,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -489,7 +611,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -604,6 +726,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -649,12 +786,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1032,7 +1173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7CAC2F-0F82-4289-AA66-82910A557688}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1064,6 +1205,257 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79254B03-63FC-4857-97F9-DDF17752BA31}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E61ED0-E1A0-4478-BDEF-59680CDA1C42}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>

</xml_diff>

<commit_message>
All integrated code without User
</commit_message>
<xml_diff>
--- a/Team14_LMS_UI_TestingSprinters/src/test/resources/TestData/LMSTestData.xlsx
+++ b/Team14_LMS_UI_TestingSprinters/src/test/resources/TestData/LMSTestData.xlsx
@@ -5,18 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumal\git\Test14_TestingSprinters_LMS_UI\Team14_LMS_UI_TestingSprinters\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balbi\git\Test14_TestingSprinters_LMS_UI\Team14_LMS_UI_TestingSprinters\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0416739-78A9-4FA5-8A6F-7C9F584AEF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F096FE3-DE5F-42EE-BE54-44CECBCDB4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="3" r:id="rId1"/>
-    <sheet name="Manage Program" sheetId="4" r:id="rId2"/>
-    <sheet name="Add Program" sheetId="5" r:id="rId3"/>
-    <sheet name="BatchSheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Batch_data" sheetId="8" r:id="rId2"/>
+    <sheet name="Manage Program" sheetId="4" r:id="rId3"/>
+    <sheet name="Add Program" sheetId="5" r:id="rId4"/>
+    <sheet name="BatchSheet" sheetId="1" r:id="rId5"/>
+    <sheet name="AddUser" sheetId="6" r:id="rId6"/>
+    <sheet name="EditUser" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="138">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -277,13 +280,190 @@
   </si>
   <si>
     <t>SDETT14</t>
+  </si>
+  <si>
+    <t>userFName</t>
+  </si>
+  <si>
+    <t>userMName</t>
+  </si>
+  <si>
+    <t>userLName</t>
+  </si>
+  <si>
+    <t>userLocationVal</t>
+  </si>
+  <si>
+    <t>userPhoneVal</t>
+  </si>
+  <si>
+    <t>userLinkedin</t>
+  </si>
+  <si>
+    <t>userRole</t>
+  </si>
+  <si>
+    <t>userRoleStatus</t>
+  </si>
+  <si>
+    <t>userVisa</t>
+  </si>
+  <si>
+    <t>userEmail</t>
+  </si>
+  <si>
+    <t>userPostGrad</t>
+  </si>
+  <si>
+    <t>userTimeZone</t>
+  </si>
+  <si>
+    <t>userComments</t>
+  </si>
+  <si>
+    <t>TestingSprintersThree</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/meena</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>TestingSprintersThree@gmail.com</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>MCA</t>
+  </si>
+  <si>
+    <t>PST</t>
+  </si>
+  <si>
+    <t>userUnderGrad</t>
+  </si>
+  <si>
+    <t>ciehwjfie9i@com</t>
+  </si>
+  <si>
+    <t>78hdu2</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Program Name</t>
+  </si>
+  <si>
+    <t>Number of Classes</t>
+  </si>
+  <si>
+    <t>Expected Message</t>
+  </si>
+  <si>
+    <t>Batch5431</t>
+  </si>
+  <si>
+    <t>WebTesting10</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>Batch  description is required</t>
+  </si>
+  <si>
+    <t>BatchTeam14</t>
+  </si>
+  <si>
+    <t>Batch Saved</t>
+  </si>
+  <si>
+    <t>Batch#Team14</t>
+  </si>
+  <si>
+    <t>SD&amp;^$@</t>
+  </si>
+  <si>
+    <t>CyPress</t>
+  </si>
+  <si>
+    <t>Error message appears</t>
+  </si>
+  <si>
+    <t>Batch Name is required</t>
+  </si>
+  <si>
+    <t>Batch1182</t>
+  </si>
+  <si>
+    <t>Batch description is required</t>
+  </si>
+  <si>
+    <t>Batch2232</t>
+  </si>
+  <si>
+    <t>Number of classes is required</t>
+  </si>
+  <si>
+    <t>Batch9232</t>
+  </si>
+  <si>
+    <t>Program Name is required</t>
+  </si>
+  <si>
+    <t>Batch9832</t>
+  </si>
+  <si>
+    <t>Status is required</t>
+  </si>
+  <si>
+    <t>TestingSprintersFour</t>
+  </si>
+  <si>
+    <t>TestingSprintersFour@gmail.com</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>TestingSprintersFive</t>
+  </si>
+  <si>
+    <t>TestingSprintersSix</t>
+  </si>
+  <si>
+    <t>TestingSprintersSeven</t>
+  </si>
+  <si>
+    <t>())</t>
+  </si>
+  <si>
+    <t>^&amp;</t>
+  </si>
+  <si>
+    <t>&lt;&gt;&lt;</t>
+  </si>
+  <si>
+    <t>(()()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +609,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -742,7 +930,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -785,8 +973,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -796,8 +985,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -831,6 +1024,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1171,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7CAC2F-0F82-4289-AA66-82910A557688}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,12 +1393,223 @@
         <v>41</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{CE202F50-70BD-4A17-BA0F-73145FA2B72D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B8CC24-FBB8-4A52-BCAD-EE5D7B826376}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{538CF139-4CE2-404F-90F6-49F6FAF0DBA9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79254B03-63FC-4857-97F9-DDF17752BA31}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1351,12 +1756,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E61ED0-E1A0-4478-BDEF-59680CDA1C42}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,12 +1860,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,4 +2304,556 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10A1DD0-E403-4BF8-94E0-7F4130A704AB}">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2222222225</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{F5550CAE-8180-442B-85F2-86AAA92B319F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9938691C-E935-4BDD-AE4D-88E4C024C0D3}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1122334455</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="8">
+        <v>4444444455</v>
+      </c>
+      <c r="N3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2244667755</v>
+      </c>
+      <c r="F4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2244667755</v>
+      </c>
+      <c r="F5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2244667755</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{BD166161-B048-4B21-8ED6-7CA0E553F087}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{92880155-AE96-4052-9BF5-5EDD9D400559}"/>
+    <hyperlink ref="J5" r:id="rId3" xr:uid="{25FA2D8C-B764-4278-82DA-96297A2F64A8}"/>
+    <hyperlink ref="J6" r:id="rId4" xr:uid="{5790B747-6686-45B8-A73C-E3AFF293C423}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>